<commit_message>
Add boundaries to catalog
</commit_message>
<xml_diff>
--- a/references/Data_Catalog.xlsx
+++ b/references/Data_Catalog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="95">
   <si>
     <t>Outcome</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>population_block_group</t>
+  </si>
+  <si>
+    <t>Cleaned</t>
+  </si>
+  <si>
+    <t>Variables aren't consistent between 2012-2017. Don't clean for now, and think about whether we need this table, or use a different table for poverty instead.</t>
   </si>
 </sst>
 </file>
@@ -647,11 +653,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +673,7 @@
     <col min="9" max="9" width="32.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -695,8 +701,11 @@
       <c r="I1" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -725,7 +734,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -754,7 +763,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -783,7 +792,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -808,8 +817,11 @@
       <c r="I5" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -832,7 +844,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -855,7 +867,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -884,7 +896,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -910,7 +922,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -936,7 +948,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -962,7 +974,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -981,6 +993,9 @@
       <c r="F12" t="s">
         <v>75</v>
       </c>
+      <c r="G12" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="H12" s="3" t="s">
         <v>69</v>
       </c>
@@ -988,7 +1003,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1007,6 +1022,9 @@
       <c r="F13" t="s">
         <v>75</v>
       </c>
+      <c r="G13" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="H13" s="3" t="s">
         <v>69</v>
       </c>
@@ -1014,7 +1032,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1040,7 +1058,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1066,7 +1084,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1092,7 +1110,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1118,7 +1136,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1146,8 +1164,11 @@
       <c r="I18" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1175,8 +1196,11 @@
       <c r="I19" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1204,8 +1228,11 @@
       <c r="I20" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1233,8 +1260,11 @@
       <c r="I21" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1260,7 +1290,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1286,7 +1316,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1314,8 +1344,11 @@
       <c r="I24" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J24" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1344,7 +1377,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1372,8 +1405,11 @@
       <c r="I26" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -1401,8 +1437,11 @@
       <c r="I27" s="3" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
Clean up tables that change over time
</commit_message>
<xml_diff>
--- a/references/Data_Catalog.xlsx
+++ b/references/Data_Catalog.xlsx
@@ -9,11 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Census" sheetId="1" r:id="rId1"/>
     <sheet name="API" sheetId="2" r:id="rId2"/>
+    <sheet name="Emp" sheetId="3" r:id="rId3"/>
+    <sheet name="Income" sheetId="4" r:id="rId4"/>
+    <sheet name="Edu" sheetId="5" r:id="rId5"/>
+    <sheet name="PovFam" sheetId="6" r:id="rId6"/>
+    <sheet name="Food" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="157">
   <si>
     <t>Outcome</t>
   </si>
@@ -310,6 +315,192 @@
   </si>
   <si>
     <t>Variables aren't consistent between 2012-2017. Don't clean for now, and think about whether we need this table, or use a different table for poverty instead.</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>One race</t>
+  </si>
+  <si>
+    <t>Pop 16+</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>AmerInd</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>PacIs</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Two race</t>
+  </si>
+  <si>
+    <t>Hisp</t>
+  </si>
+  <si>
+    <t>Non-Hisp</t>
+  </si>
+  <si>
+    <t>Pop 20-64</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Female with children under 6</t>
+  </si>
+  <si>
+    <t>Below poverty</t>
+  </si>
+  <si>
+    <t>Edu: less HS</t>
+  </si>
+  <si>
+    <t>Edu: pop 25=64</t>
+  </si>
+  <si>
+    <t>Edu: HS</t>
+  </si>
+  <si>
+    <t>Edu: college</t>
+  </si>
+  <si>
+    <t>Edu: ba</t>
+  </si>
+  <si>
+    <t>Total HH</t>
+  </si>
+  <si>
+    <t>Checked API</t>
+  </si>
+  <si>
+    <t>Downloaded Again</t>
+  </si>
+  <si>
+    <t>Good as is</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>dropped C03, replaced S3</t>
+  </si>
+  <si>
+    <t>pop 25+</t>
+  </si>
+  <si>
+    <t>Less than 9</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>HS 9-12</t>
+  </si>
+  <si>
+    <t>College</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>Graduate</t>
+  </si>
+  <si>
+    <t>Pct HS</t>
+  </si>
+  <si>
+    <t>Pct BA</t>
+  </si>
+  <si>
+    <t>HS: pov</t>
+  </si>
+  <si>
+    <t>College: pov</t>
+  </si>
+  <si>
+    <t>BA: pov</t>
+  </si>
+  <si>
+    <t>Pop 25+ Less HS: pov</t>
+  </si>
+  <si>
+    <t>Pop 25+ with earnings: med earnings</t>
+  </si>
+  <si>
+    <t>Pop 25+ HS: med earnings</t>
+  </si>
+  <si>
+    <t>Pop 25+ LHS: med earnings</t>
+  </si>
+  <si>
+    <t>Pop 25+ college med earnings</t>
+  </si>
+  <si>
+    <t>Pop 25+ BA med earnings</t>
+  </si>
+  <si>
+    <t>Pop 25+ Grad med earnings</t>
+  </si>
+  <si>
+    <t>families below pov</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>C02</t>
+  </si>
+  <si>
+    <t>hh</t>
+  </si>
+  <si>
+    <t>below pov</t>
+  </si>
+  <si>
+    <t>med hh income</t>
+  </si>
+  <si>
+    <t>S2301</t>
+  </si>
+  <si>
+    <t>S2201</t>
+  </si>
+  <si>
+    <t>S1702</t>
+  </si>
+  <si>
+    <t>S1501</t>
+  </si>
+  <si>
+    <t>S1903</t>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>Edu: pop 25-64</t>
   </si>
 </sst>
 </file>
@@ -362,7 +553,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -372,6 +563,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -653,11 +845,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +865,7 @@
     <col min="9" max="9" width="32.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -704,8 +896,14 @@
       <c r="J1" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -734,7 +932,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -763,7 +961,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -792,7 +990,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -820,8 +1018,14 @@
       <c r="J5" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -844,7 +1048,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -867,7 +1071,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -890,13 +1094,14 @@
         <v>74</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -916,13 +1121,13 @@
         <v>76</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -947,8 +1152,14 @@
       <c r="I10" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -973,8 +1184,14 @@
       <c r="I11" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1002,8 +1219,9 @@
       <c r="I12" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1032,7 +1250,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1057,8 +1275,14 @@
       <c r="I14" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1083,8 +1307,14 @@
       <c r="I15" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1109,8 +1339,14 @@
       <c r="I16" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1136,7 +1372,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1167,8 +1403,14 @@
       <c r="J18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1199,8 +1441,14 @@
       <c r="J19" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1231,8 +1479,14 @@
       <c r="J20" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1263,8 +1517,14 @@
       <c r="J21" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1290,7 +1550,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1316,7 +1576,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1348,7 +1608,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1377,7 +1637,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1409,7 +1669,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -1441,7 +1701,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1478,7 +1738,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,4 +1769,2297 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1">
+        <v>2010</v>
+      </c>
+      <c r="D1">
+        <v>2011</v>
+      </c>
+      <c r="E1">
+        <v>2012</v>
+      </c>
+      <c r="F1">
+        <v>2013</v>
+      </c>
+      <c r="G1">
+        <v>2014</v>
+      </c>
+      <c r="H1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1">
+        <v>2015</v>
+      </c>
+      <c r="K1">
+        <v>2016</v>
+      </c>
+      <c r="L1">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" t="s">
+        <v>69</v>
+      </c>
+      <c r="L6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8">
+        <v>16</v>
+      </c>
+      <c r="J8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" t="s">
+        <v>69</v>
+      </c>
+      <c r="L9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I10">
+        <v>18</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>106</v>
+      </c>
+      <c r="I11">
+        <v>19</v>
+      </c>
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" t="s">
+        <v>107</v>
+      </c>
+      <c r="I12">
+        <v>20</v>
+      </c>
+      <c r="J12" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I13">
+        <v>21</v>
+      </c>
+      <c r="J13" t="s">
+        <v>69</v>
+      </c>
+      <c r="K13" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I14">
+        <v>22</v>
+      </c>
+      <c r="J14" t="s">
+        <v>69</v>
+      </c>
+      <c r="K14" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" t="s">
+        <v>110</v>
+      </c>
+      <c r="I15">
+        <v>23</v>
+      </c>
+      <c r="J15" t="s">
+        <v>69</v>
+      </c>
+      <c r="K15" t="s">
+        <v>69</v>
+      </c>
+      <c r="L15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" t="s">
+        <v>111</v>
+      </c>
+      <c r="I16">
+        <v>25</v>
+      </c>
+      <c r="J16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K16" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" t="s">
+        <v>112</v>
+      </c>
+      <c r="I17">
+        <v>28</v>
+      </c>
+      <c r="J17" t="s">
+        <v>69</v>
+      </c>
+      <c r="K17" t="s">
+        <v>69</v>
+      </c>
+      <c r="L17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" t="s">
+        <v>156</v>
+      </c>
+      <c r="I18">
+        <v>31</v>
+      </c>
+      <c r="J18" t="s">
+        <v>69</v>
+      </c>
+      <c r="K18" t="s">
+        <v>69</v>
+      </c>
+      <c r="L18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" t="s">
+        <v>113</v>
+      </c>
+      <c r="I19">
+        <v>32</v>
+      </c>
+      <c r="J19" t="s">
+        <v>69</v>
+      </c>
+      <c r="K19" t="s">
+        <v>69</v>
+      </c>
+      <c r="L19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" t="s">
+        <v>115</v>
+      </c>
+      <c r="I20">
+        <v>33</v>
+      </c>
+      <c r="J20" t="s">
+        <v>69</v>
+      </c>
+      <c r="K20" t="s">
+        <v>69</v>
+      </c>
+      <c r="L20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21" t="s">
+        <v>116</v>
+      </c>
+      <c r="I21">
+        <v>34</v>
+      </c>
+      <c r="J21" t="s">
+        <v>69</v>
+      </c>
+      <c r="K21" t="s">
+        <v>69</v>
+      </c>
+      <c r="L21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22" t="s">
+        <v>69</v>
+      </c>
+      <c r="H22" t="s">
+        <v>117</v>
+      </c>
+      <c r="I22">
+        <v>35</v>
+      </c>
+      <c r="J22" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22" t="s">
+        <v>69</v>
+      </c>
+      <c r="L22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1">
+        <v>2010</v>
+      </c>
+      <c r="D1">
+        <v>2011</v>
+      </c>
+      <c r="E1">
+        <v>2012</v>
+      </c>
+      <c r="F1">
+        <v>2013</v>
+      </c>
+      <c r="G1">
+        <v>2014</v>
+      </c>
+      <c r="H1">
+        <v>2015</v>
+      </c>
+      <c r="I1">
+        <v>2016</v>
+      </c>
+      <c r="J1">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1">
+        <v>2010</v>
+      </c>
+      <c r="D1">
+        <v>2011</v>
+      </c>
+      <c r="E1">
+        <v>2012</v>
+      </c>
+      <c r="F1">
+        <v>2013</v>
+      </c>
+      <c r="G1">
+        <v>2014</v>
+      </c>
+      <c r="H1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1">
+        <v>2015</v>
+      </c>
+      <c r="K1">
+        <v>2016</v>
+      </c>
+      <c r="L1">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I3">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+      <c r="J5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" t="s">
+        <v>128</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" t="s">
+        <v>69</v>
+      </c>
+      <c r="L6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I7">
+        <v>11</v>
+      </c>
+      <c r="J7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" t="s">
+        <v>130</v>
+      </c>
+      <c r="I8">
+        <v>12</v>
+      </c>
+      <c r="J8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I9">
+        <v>13</v>
+      </c>
+      <c r="J9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" t="s">
+        <v>69</v>
+      </c>
+      <c r="L9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s">
+        <v>132</v>
+      </c>
+      <c r="I10">
+        <v>14</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>133</v>
+      </c>
+      <c r="I11">
+        <v>15</v>
+      </c>
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I12">
+        <v>55</v>
+      </c>
+      <c r="J12" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" t="s">
+        <v>134</v>
+      </c>
+      <c r="I13">
+        <v>56</v>
+      </c>
+      <c r="J13" t="s">
+        <v>69</v>
+      </c>
+      <c r="K13" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" t="s">
+        <v>135</v>
+      </c>
+      <c r="I14">
+        <v>57</v>
+      </c>
+      <c r="J14" t="s">
+        <v>69</v>
+      </c>
+      <c r="K14" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" t="s">
+        <v>136</v>
+      </c>
+      <c r="I15">
+        <v>58</v>
+      </c>
+      <c r="J15" t="s">
+        <v>69</v>
+      </c>
+      <c r="K15" t="s">
+        <v>69</v>
+      </c>
+      <c r="L15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" t="s">
+        <v>138</v>
+      </c>
+      <c r="I16">
+        <v>59</v>
+      </c>
+      <c r="J16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K16" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" t="s">
+        <v>140</v>
+      </c>
+      <c r="I17">
+        <v>60</v>
+      </c>
+      <c r="J17" t="s">
+        <v>69</v>
+      </c>
+      <c r="K17" t="s">
+        <v>69</v>
+      </c>
+      <c r="L17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" t="s">
+        <v>139</v>
+      </c>
+      <c r="I18">
+        <v>61</v>
+      </c>
+      <c r="J18" t="s">
+        <v>69</v>
+      </c>
+      <c r="K18" t="s">
+        <v>69</v>
+      </c>
+      <c r="L18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B19">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" t="s">
+        <v>141</v>
+      </c>
+      <c r="I19">
+        <v>62</v>
+      </c>
+      <c r="J19" t="s">
+        <v>69</v>
+      </c>
+      <c r="K19" t="s">
+        <v>69</v>
+      </c>
+      <c r="L19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I20">
+        <v>63</v>
+      </c>
+      <c r="J20" t="s">
+        <v>69</v>
+      </c>
+      <c r="K20" t="s">
+        <v>69</v>
+      </c>
+      <c r="L20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21" t="s">
+        <v>143</v>
+      </c>
+      <c r="I21">
+        <v>64</v>
+      </c>
+      <c r="J21" t="s">
+        <v>69</v>
+      </c>
+      <c r="K21" t="s">
+        <v>69</v>
+      </c>
+      <c r="L21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1">
+        <v>2010</v>
+      </c>
+      <c r="D1">
+        <v>2011</v>
+      </c>
+      <c r="E1">
+        <v>2012</v>
+      </c>
+      <c r="F1">
+        <v>2013</v>
+      </c>
+      <c r="G1">
+        <v>2014</v>
+      </c>
+      <c r="H1">
+        <v>2015</v>
+      </c>
+      <c r="I1">
+        <v>2016</v>
+      </c>
+      <c r="J1">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1">
+        <v>2010</v>
+      </c>
+      <c r="D1">
+        <v>2011</v>
+      </c>
+      <c r="E1">
+        <v>2012</v>
+      </c>
+      <c r="F1">
+        <v>2013</v>
+      </c>
+      <c r="G1">
+        <v>2014</v>
+      </c>
+      <c r="H1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1">
+        <v>2015</v>
+      </c>
+      <c r="K1">
+        <v>2016</v>
+      </c>
+      <c r="L1">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" t="s">
+        <v>148</v>
+      </c>
+      <c r="I3">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="I4">
+        <v>34</v>
+      </c>
+      <c r="J4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>146</v>
+      </c>
+      <c r="H7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adjust values to percents
</commit_message>
<xml_diff>
--- a/references/Data_Catalog.xlsx
+++ b/references/Data_Catalog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Census" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Edu" sheetId="5" r:id="rId5"/>
     <sheet name="PovFam" sheetId="6" r:id="rId6"/>
     <sheet name="Food" sheetId="7" r:id="rId7"/>
+    <sheet name="PubAssist" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="167">
   <si>
     <t>Outcome</t>
   </si>
@@ -501,6 +502,36 @@
   </si>
   <si>
     <t>Edu: pop 25-64</t>
+  </si>
+  <si>
+    <t>C04</t>
+  </si>
+  <si>
+    <t>unemployment rate (%)</t>
+  </si>
+  <si>
+    <t>employment/population ratio (%)</t>
+  </si>
+  <si>
+    <t>labor force participation rate (%)</t>
+  </si>
+  <si>
+    <t>total number</t>
+  </si>
+  <si>
+    <t>B19058</t>
+  </si>
+  <si>
+    <t>total hh</t>
+  </si>
+  <si>
+    <t>hh with public assistance</t>
+  </si>
+  <si>
+    <t>number of hh</t>
+  </si>
+  <si>
+    <t>derive: % of hh with public assistance</t>
   </si>
 </sst>
 </file>
@@ -848,8 +879,8 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1773,10 +1804,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2593,6 +2624,38 @@
         <v>69</v>
       </c>
     </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>155</v>
+      </c>
+      <c r="B26" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>157</v>
+      </c>
+      <c r="B27" t="s">
+        <v>158</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2603,7 +2666,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2974,8 +3037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3790,8 +3853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4062,4 +4125,126 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1">
+        <v>2010</v>
+      </c>
+      <c r="D1">
+        <v>2011</v>
+      </c>
+      <c r="E1">
+        <v>2012</v>
+      </c>
+      <c r="F1">
+        <v>2013</v>
+      </c>
+      <c r="G1">
+        <v>2014</v>
+      </c>
+      <c r="H1">
+        <v>2015</v>
+      </c>
+      <c r="I1">
+        <v>2016</v>
+      </c>
+      <c r="J1">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Check for consistent values over time
</commit_message>
<xml_diff>
--- a/references/Data_Catalog.xlsx
+++ b/references/Data_Catalog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Census" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="172">
   <si>
     <t>Outcome</t>
   </si>
@@ -535,6 +535,18 @@
   </si>
   <si>
     <t>hh that receive food stamps</t>
+  </si>
+  <si>
+    <t>2010-2016</t>
+  </si>
+  <si>
+    <t>median hh income</t>
+  </si>
+  <si>
+    <t>% by race</t>
+  </si>
+  <si>
+    <t>number of hh by race</t>
   </si>
 </sst>
 </file>
@@ -2666,10 +2678,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3028,7 +3040,54 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>121</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>145</v>
+      </c>
+      <c r="B20" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>155</v>
+      </c>
+      <c r="B22" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3951,7 +4010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Re-download education S1501 table
</commit_message>
<xml_diff>
--- a/references/Data_Catalog.xlsx
+++ b/references/Data_Catalog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Census" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="176">
   <si>
     <t>Outcome</t>
   </si>
@@ -547,6 +547,18 @@
   </si>
   <si>
     <t>number of hh by race</t>
+  </si>
+  <si>
+    <t>2010-2014</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>2015-2017</t>
+  </si>
+  <si>
+    <t>same col is blank</t>
   </si>
 </sst>
 </file>
@@ -2680,7 +2692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -3097,15 +3109,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="34.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3904,6 +3917,60 @@
       </c>
       <c r="L21" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28">
+        <v>14</v>
+      </c>
+      <c r="C28" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get consistent values over time
</commit_message>
<xml_diff>
--- a/references/Data_Catalog.xlsx
+++ b/references/Data_Catalog.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="175">
   <si>
     <t>Outcome</t>
   </si>
@@ -556,9 +556,6 @@
   </si>
   <si>
     <t>2015-2017</t>
-  </si>
-  <si>
-    <t>same col is blank</t>
   </si>
 </sst>
 </file>
@@ -3109,10 +3106,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3934,6 +3931,9 @@
       <c r="C25" t="s">
         <v>173</v>
       </c>
+      <c r="D25" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -3945,32 +3945,153 @@
       <c r="C26" t="s">
         <v>173</v>
       </c>
+      <c r="D26" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>174</v>
+        <v>137</v>
+      </c>
+      <c r="B27">
+        <v>28</v>
+      </c>
+      <c r="C27" t="s">
+        <v>173</v>
+      </c>
+      <c r="D27" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B28">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>175</v>
+        <v>173</v>
+      </c>
+      <c r="D28" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>173</v>
+      </c>
+      <c r="D29" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30">
+        <v>31</v>
+      </c>
+      <c r="C30" t="s">
+        <v>173</v>
+      </c>
+      <c r="D30" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>173</v>
+      </c>
+      <c r="D33" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>133</v>
       </c>
-      <c r="B29">
+      <c r="B34">
         <v>15</v>
       </c>
-      <c r="C29" t="s">
-        <v>175</v>
+      <c r="C34" t="s">
+        <v>173</v>
+      </c>
+      <c r="D34" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>137</v>
+      </c>
+      <c r="B35">
+        <v>55</v>
+      </c>
+      <c r="C35" t="s">
+        <v>173</v>
+      </c>
+      <c r="D35" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36">
+        <v>56</v>
+      </c>
+      <c r="C36" t="s">
+        <v>173</v>
+      </c>
+      <c r="D36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37">
+        <v>57</v>
+      </c>
+      <c r="C37" t="s">
+        <v>173</v>
+      </c>
+      <c r="D37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38">
+        <v>58</v>
+      </c>
+      <c r="C38" t="s">
+        <v>173</v>
+      </c>
+      <c r="D38" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Download income range tables from ACS
</commit_message>
<xml_diff>
--- a/references/Data_Catalog.xlsx
+++ b/references/Data_Catalog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Census" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="216">
   <si>
     <t>Outcome</t>
   </si>
@@ -556,6 +556,129 @@
   </si>
   <si>
     <t>2015-2017</t>
+  </si>
+  <si>
+    <t>B19001</t>
+  </si>
+  <si>
+    <t>Less than $10k</t>
+  </si>
+  <si>
+    <t>10k-14k</t>
+  </si>
+  <si>
+    <t>15-19k</t>
+  </si>
+  <si>
+    <t>20-24k</t>
+  </si>
+  <si>
+    <t>25-29k</t>
+  </si>
+  <si>
+    <t>30-34k</t>
+  </si>
+  <si>
+    <t>40-44k</t>
+  </si>
+  <si>
+    <t>45-49k</t>
+  </si>
+  <si>
+    <t>35-39k</t>
+  </si>
+  <si>
+    <t>50-59k</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>60-74k</t>
+  </si>
+  <si>
+    <t>75-99k</t>
+  </si>
+  <si>
+    <t>100-124k</t>
+  </si>
+  <si>
+    <t>125-149k</t>
+  </si>
+  <si>
+    <t>150-199k</t>
+  </si>
+  <si>
+    <t>200k or more</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>amerind</t>
+  </si>
+  <si>
+    <t>asian</t>
+  </si>
+  <si>
+    <t>pacis</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>race2</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>nonhisp</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>hisp</t>
+  </si>
+  <si>
+    <t>household income by race/ethnicity and income range</t>
+  </si>
+  <si>
+    <t>ACS Household Income in Past 12 Months (B19001)</t>
+  </si>
+  <si>
+    <t>ACS 5 Yr</t>
+  </si>
+  <si>
+    <t>income_range_tract</t>
+  </si>
+  <si>
+    <t>use the ranges to aggregate median hh income up to larger geographies</t>
   </si>
 </sst>
 </file>
@@ -587,12 +710,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -608,7 +737,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -619,6 +748,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -900,11 +1030,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,26 +1234,27 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>211</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>17</v>
+        <v>212</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>79</v>
+      <c r="G7" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1131,10 +1262,10 @@
         <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>67</v>
@@ -1145,23 +1276,16 @@
       <c r="F8" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="H8" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>18</v>
@@ -1175,19 +1299,23 @@
       <c r="F9" t="s">
         <v>76</v>
       </c>
+      <c r="G9" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="H9" s="3" t="s">
         <v>79</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>18</v>
@@ -1202,24 +1330,18 @@
         <v>76</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>18</v>
@@ -1246,15 +1368,15 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>67</v>
@@ -1263,25 +1385,27 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>69</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K12" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>28</v>
@@ -1304,16 +1428,17 @@
       <c r="I13" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>67</v>
@@ -1322,30 +1447,27 @@
         <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>69</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>67</v>
@@ -1360,7 +1482,7 @@
         <v>69</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>69</v>
@@ -1374,7 +1496,7 @@
         <v>26</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>31</v>
@@ -1401,15 +1523,15 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>67</v>
@@ -1420,11 +1542,17 @@
       <c r="F17" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="H17" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -1432,7 +1560,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>39</v>
@@ -1449,20 +1577,8 @@
       <c r="G18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H18" t="s">
-        <v>69</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J18" t="s">
-        <v>69</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="L18" t="s">
-        <v>122</v>
+      <c r="H18" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -1470,7 +1586,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>39</v>
@@ -1508,7 +1624,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>39</v>
@@ -1546,7 +1662,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>39</v>
@@ -1579,15 +1695,15 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>67</v>
@@ -1599,24 +1715,36 @@
         <v>76</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="H22" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J22" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1625,7 +1753,7 @@
         <v>76</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>79</v>
@@ -1636,10 +1764,10 @@
         <v>26</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>14</v>
@@ -1651,27 +1779,21 @@
         <v>76</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>14</v>
@@ -1683,24 +1805,27 @@
         <v>76</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>69</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>14</v>
@@ -1712,27 +1837,24 @@
         <v>76</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>69</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J26" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>14</v>
@@ -1744,41 +1866,73 @@
         <v>76</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H27" t="s">
         <v>69</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J27" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" t="s">
+        <v>69</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" t="s">
         <v>64</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" t="s">
         <v>65</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="I29" s="3" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1830,9 +1984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1840,7 +1992,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>150</v>
       </c>
       <c r="B1" t="s">
@@ -2687,16 +2839,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>154</v>
       </c>
       <c r="B1" t="s">
@@ -3073,12 +3228,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2017</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>145</v>
       </c>
@@ -3086,17 +3241,665 @@
         <v>165</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>155</v>
       </c>
       <c r="B22" t="s">
         <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26">
+        <v>2010</v>
+      </c>
+      <c r="D26">
+        <v>2011</v>
+      </c>
+      <c r="E26">
+        <v>2012</v>
+      </c>
+      <c r="F26">
+        <v>2013</v>
+      </c>
+      <c r="G26">
+        <v>2014</v>
+      </c>
+      <c r="H26">
+        <v>2015</v>
+      </c>
+      <c r="I26">
+        <v>2016</v>
+      </c>
+      <c r="J26">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>186</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" t="s">
+        <v>69</v>
+      </c>
+      <c r="H27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I27" t="s">
+        <v>69</v>
+      </c>
+      <c r="J27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>176</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" t="s">
+        <v>69</v>
+      </c>
+      <c r="H28" t="s">
+        <v>69</v>
+      </c>
+      <c r="I28" t="s">
+        <v>69</v>
+      </c>
+      <c r="J28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>177</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" t="s">
+        <v>69</v>
+      </c>
+      <c r="H29" t="s">
+        <v>69</v>
+      </c>
+      <c r="I29" t="s">
+        <v>69</v>
+      </c>
+      <c r="J29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>178</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" t="s">
+        <v>69</v>
+      </c>
+      <c r="H30" t="s">
+        <v>69</v>
+      </c>
+      <c r="I30" t="s">
+        <v>69</v>
+      </c>
+      <c r="J30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>179</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" t="s">
+        <v>69</v>
+      </c>
+      <c r="H31" t="s">
+        <v>69</v>
+      </c>
+      <c r="I31" t="s">
+        <v>69</v>
+      </c>
+      <c r="J31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>180</v>
+      </c>
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" t="s">
+        <v>69</v>
+      </c>
+      <c r="H32" t="s">
+        <v>69</v>
+      </c>
+      <c r="I32" t="s">
+        <v>69</v>
+      </c>
+      <c r="J32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" t="s">
+        <v>69</v>
+      </c>
+      <c r="F33" t="s">
+        <v>69</v>
+      </c>
+      <c r="G33" t="s">
+        <v>69</v>
+      </c>
+      <c r="H33" t="s">
+        <v>69</v>
+      </c>
+      <c r="I33" t="s">
+        <v>69</v>
+      </c>
+      <c r="J33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>184</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" t="s">
+        <v>69</v>
+      </c>
+      <c r="F34" t="s">
+        <v>69</v>
+      </c>
+      <c r="G34" t="s">
+        <v>69</v>
+      </c>
+      <c r="H34" t="s">
+        <v>69</v>
+      </c>
+      <c r="I34" t="s">
+        <v>69</v>
+      </c>
+      <c r="J34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>182</v>
+      </c>
+      <c r="B35">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35" t="s">
+        <v>69</v>
+      </c>
+      <c r="G35" t="s">
+        <v>69</v>
+      </c>
+      <c r="H35" t="s">
+        <v>69</v>
+      </c>
+      <c r="I35" t="s">
+        <v>69</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>183</v>
+      </c>
+      <c r="B36">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" t="s">
+        <v>69</v>
+      </c>
+      <c r="F36" t="s">
+        <v>69</v>
+      </c>
+      <c r="G36" t="s">
+        <v>69</v>
+      </c>
+      <c r="H36" t="s">
+        <v>69</v>
+      </c>
+      <c r="I36" t="s">
+        <v>69</v>
+      </c>
+      <c r="J36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>185</v>
+      </c>
+      <c r="B37">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" t="s">
+        <v>69</v>
+      </c>
+      <c r="F37" t="s">
+        <v>69</v>
+      </c>
+      <c r="G37" t="s">
+        <v>69</v>
+      </c>
+      <c r="H37" t="s">
+        <v>69</v>
+      </c>
+      <c r="I37" t="s">
+        <v>69</v>
+      </c>
+      <c r="J37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>187</v>
+      </c>
+      <c r="B38">
+        <v>12</v>
+      </c>
+      <c r="C38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" t="s">
+        <v>69</v>
+      </c>
+      <c r="F38" t="s">
+        <v>69</v>
+      </c>
+      <c r="G38" t="s">
+        <v>69</v>
+      </c>
+      <c r="H38" t="s">
+        <v>69</v>
+      </c>
+      <c r="I38" t="s">
+        <v>69</v>
+      </c>
+      <c r="J38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>188</v>
+      </c>
+      <c r="B39">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" t="s">
+        <v>69</v>
+      </c>
+      <c r="F39" t="s">
+        <v>69</v>
+      </c>
+      <c r="G39" t="s">
+        <v>69</v>
+      </c>
+      <c r="H39" t="s">
+        <v>69</v>
+      </c>
+      <c r="I39" t="s">
+        <v>69</v>
+      </c>
+      <c r="J39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>189</v>
+      </c>
+      <c r="B40">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" t="s">
+        <v>69</v>
+      </c>
+      <c r="F40" t="s">
+        <v>69</v>
+      </c>
+      <c r="G40" t="s">
+        <v>69</v>
+      </c>
+      <c r="H40" t="s">
+        <v>69</v>
+      </c>
+      <c r="I40" t="s">
+        <v>69</v>
+      </c>
+      <c r="J40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>190</v>
+      </c>
+      <c r="B41">
+        <v>15</v>
+      </c>
+      <c r="C41" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" t="s">
+        <v>69</v>
+      </c>
+      <c r="F41" t="s">
+        <v>69</v>
+      </c>
+      <c r="G41" t="s">
+        <v>69</v>
+      </c>
+      <c r="H41" t="s">
+        <v>69</v>
+      </c>
+      <c r="I41" t="s">
+        <v>69</v>
+      </c>
+      <c r="J41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>191</v>
+      </c>
+      <c r="B42">
+        <v>16</v>
+      </c>
+      <c r="C42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" t="s">
+        <v>69</v>
+      </c>
+      <c r="E42" t="s">
+        <v>69</v>
+      </c>
+      <c r="F42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G42" t="s">
+        <v>69</v>
+      </c>
+      <c r="H42" t="s">
+        <v>69</v>
+      </c>
+      <c r="I42" t="s">
+        <v>69</v>
+      </c>
+      <c r="J42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>192</v>
+      </c>
+      <c r="B43">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E43" t="s">
+        <v>69</v>
+      </c>
+      <c r="F43" t="s">
+        <v>69</v>
+      </c>
+      <c r="G43" t="s">
+        <v>69</v>
+      </c>
+      <c r="H43" t="s">
+        <v>69</v>
+      </c>
+      <c r="I43" t="s">
+        <v>69</v>
+      </c>
+      <c r="J43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>193</v>
+      </c>
+      <c r="B46" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>194</v>
+      </c>
+      <c r="B47" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>195</v>
+      </c>
+      <c r="B48" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>196</v>
+      </c>
+      <c r="B49" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>197</v>
+      </c>
+      <c r="B50" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>198</v>
+      </c>
+      <c r="B51" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>205</v>
+      </c>
+      <c r="B52" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>207</v>
+      </c>
+      <c r="B53" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>209</v>
+      </c>
+      <c r="B54" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3108,8 +3911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3119,7 +3922,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>153</v>
       </c>
       <c r="B1" t="s">
@@ -4103,14 +4906,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>152</v>
       </c>
       <c r="B1" t="s">
@@ -4198,14 +4999,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>151</v>
       </c>
       <c r="B1" t="s">
@@ -4393,14 +5192,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>162</v>
       </c>
       <c r="B1" t="s">

</xml_diff>

<commit_message>
Download more ACS tables
</commit_message>
<xml_diff>
--- a/references/Data_Catalog.xlsx
+++ b/references/Data_Catalog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="255">
   <si>
     <t>Outcome</t>
   </si>
@@ -764,6 +764,36 @@
   </si>
   <si>
     <t>poverty status by sex</t>
+  </si>
+  <si>
+    <t>health insurance coverage</t>
+  </si>
+  <si>
+    <t>Health Insurance</t>
+  </si>
+  <si>
+    <t>DP03</t>
+  </si>
+  <si>
+    <t>Selected Economic Characteristics (DP03)</t>
+  </si>
+  <si>
+    <t>ACS 5 yr Profile</t>
+  </si>
+  <si>
+    <t>health_insurance_tract</t>
+  </si>
+  <si>
+    <t>with health coverage</t>
+  </si>
+  <si>
+    <t>private insurance</t>
+  </si>
+  <si>
+    <t>public coverage</t>
+  </si>
+  <si>
+    <t>no coverage</t>
   </si>
 </sst>
 </file>
@@ -828,301 +858,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="60">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0EAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE2EFDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAF2DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAEDBC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCBF0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0EAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE2EFDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAF2DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAEDBC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCBF0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0EAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE2EFDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAF2DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAEDBC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCBF0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0EAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE2EFDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAF2DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAEDBC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCBF0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0EAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE2EFDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAF2DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAEDBC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCBF0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0EAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE2EFDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAF2DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAEDBC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCBF0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0EAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE2EFDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAF2DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAEDBC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCBF0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <fill>
         <patternFill>
@@ -1539,11 +1275,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2408,25 +2144,72 @@
         <v>70</v>
       </c>
     </row>
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2:J28">
-    <cfRule type="expression" dxfId="53" priority="1">
+    <cfRule type="expression" dxfId="11" priority="31">
       <formula xml:space="preserve"> $A2 = "population"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="3">
+    <cfRule type="expression" dxfId="10" priority="33">
       <formula>$A2 = "quality of life"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="4">
+    <cfRule type="expression" dxfId="9" priority="34">
       <formula>$A2 = "education"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="5">
+    <cfRule type="expression" dxfId="8" priority="35">
       <formula>$A2 = "poverty"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="6">
+    <cfRule type="expression" dxfId="7" priority="36">
       <formula>$A2 = "income"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="7">
+    <cfRule type="expression" dxfId="6" priority="37">
       <formula>$A2 = "employment"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:J29">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula xml:space="preserve"> $A29 = "population"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>$A29 = "quality of life"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$A29 = "education"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$A29 = "poverty"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="5">
+      <formula>$A29 = "income"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="6">
+      <formula>$A29 = "employment"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4847,8 +4630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5843,7 +5626,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="A20" sqref="A20:J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6736,10 +6519,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7041,6 +6824,203 @@
         <v>138</v>
       </c>
     </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20">
+        <v>2010</v>
+      </c>
+      <c r="D20">
+        <v>2011</v>
+      </c>
+      <c r="E20">
+        <v>2012</v>
+      </c>
+      <c r="F20">
+        <v>2013</v>
+      </c>
+      <c r="G20">
+        <v>2014</v>
+      </c>
+      <c r="H20">
+        <v>2015</v>
+      </c>
+      <c r="I20">
+        <v>2016</v>
+      </c>
+      <c r="J20">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>237</v>
+      </c>
+      <c r="B21">
+        <v>95</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" t="s">
+        <v>48</v>
+      </c>
+      <c r="J21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>251</v>
+      </c>
+      <c r="B22">
+        <v>96</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" t="s">
+        <v>48</v>
+      </c>
+      <c r="J22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B23">
+        <v>97</v>
+      </c>
+      <c r="C23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" t="s">
+        <v>48</v>
+      </c>
+      <c r="J23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>253</v>
+      </c>
+      <c r="B24">
+        <v>98</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" t="s">
+        <v>48</v>
+      </c>
+      <c r="J24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>254</v>
+      </c>
+      <c r="B25">
+        <v>99</v>
+      </c>
+      <c r="C25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" t="s">
+        <v>48</v>
+      </c>
+      <c r="J25" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>